<commit_message>
Sprint 4 finalizado - Seguir con mejoras y fix
</commit_message>
<xml_diff>
--- a/assets/docs/export.xlsx
+++ b/assets/docs/export.xlsx
@@ -11,46 +11,64 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Identificador</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>NOTA DE PEDIDO</t>
+  </si>
+  <si>
+    <t>A PROVEEDORES</t>
+  </si>
+  <si>
+    <t>Numero</t>
+  </si>
+  <si>
+    <t>Proveedor</t>
   </si>
   <si>
     <t>Fecha</t>
   </si>
   <si>
-    <t>Área</t>
-  </si>
-  <si>
     <t>Solicitante</t>
   </si>
   <si>
-    <t>2022-08-01 00:00:00</t>
-  </si>
-  <si>
-    <t>Area 3</t>
+    <t>Proveedor 3</t>
+  </si>
+  <si>
+    <t>17/ago./22</t>
   </si>
   <si>
     <t>Ivan Villan</t>
   </si>
   <si>
+    <t>PAÑOL</t>
+  </si>
+  <si>
+    <t>DETALLE  DEL</t>
+  </si>
+  <si>
+    <t>PEDIDO</t>
+  </si>
+  <si>
     <t>Cantidad</t>
   </si>
   <si>
     <t>Producto</t>
   </si>
   <si>
-    <t>Producto 1</t>
-  </si>
-  <si>
-    <t>Producto 4</t>
+    <t>Dato</t>
+  </si>
+  <si>
+    <t>New product</t>
+  </si>
+  <si>
+    <t>Categoria 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -58,16 +76,75 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <color rgb="FFFFFF"/>
+      <family val="2"/>
+      <sz val="18"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FFFFFF"/>
+      <family val="2"/>
+      <sz val="24"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FFFFFF"/>
+      <family val="2"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FFFFFF"/>
+      <family val="2"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="000000"/>
+      <family val="2"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="424851"/>
+        <bgColor rgb="424851"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C33C01"/>
+        <bgColor rgb="C33C01"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C0C0C0"/>
+        <bgColor rgb="C0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="8FD24C"/>
+        <bgColor rgb="8FD24C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -75,12 +152,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -102,10 +230,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>90000</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1114425" cy="514350"/>
     <xdr:pic>
@@ -143,17 +271,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="header" displayName="header" ref="C1:F2" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="C1:F2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="header" displayName="header" ref="A6:D7" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A6:D7">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="Identificador" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Fecha" totalsRowFunction="none"/>
-    <tableColumn id="3" name="Área" totalsRowFunction="none"/>
+    <tableColumn id="1" name="Numero" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Proveedor" totalsRowFunction="none"/>
+    <tableColumn id="3" name="Fecha" totalsRowFunction="none"/>
     <tableColumn id="4" name="Solicitante" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -161,14 +289,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" name="products" displayName="products" ref="A4:B6" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A4:B6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" name="products" displayName="products" ref="A10:C11" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A10:C11">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="2">
+  <tableColumns count="3">
     <tableColumn id="1" name="Cantidad" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Producto" totalsRowFunction="none"/>
+    <tableColumn id="3" name="Dato" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -496,56 +626,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:D11"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="15" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D2" t="s">
+      <c r="C6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>19</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D7" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11" t="s">
         <v>10</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="13"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>